<commit_message>
Adding Office Tools Files
</commit_message>
<xml_diff>
--- a/SF4630_UPDATEDEXCEL ASSIGNMENT.xlsx
+++ b/SF4630_UPDATEDEXCEL ASSIGNMENT.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PriyadharshiniKesava\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syncfusion-my.sharepoint.com/personal/priyadharshini_kesavan_syncfusion_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{661C4D21-C8EF-49E7-9054-F995C5BC9C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62A7FE9C-CE41-48F0-82C4-ADEAE0DB69E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0B057EDB-AAC2-4DD5-814A-814347E46EF7}"/>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{426DCCCC-1DDF-425F-B5D8-747347B22089}"/>
+    <workbookView xWindow="432" yWindow="84" windowWidth="22608" windowHeight="12156" activeTab="2" xr2:uid="{0B057EDB-AAC2-4DD5-814A-814347E46EF7}"/>
+    <workbookView xWindow="432" yWindow="804" windowWidth="22608" windowHeight="12156" activeTab="2" xr2:uid="{426DCCCC-1DDF-425F-B5D8-747347B22089}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
@@ -89267,6 +89267,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5637b85f-05ae-42d6-879b-f626b8425ad6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="018a9009-0ad3-4c01-a706-708408b93adc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB018D4A967C3C48AE74E117DC16159E" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="07acbd51033d96003dbeaab03acf2e1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="018a9009-0ad3-4c01-a706-708408b93adc" xmlns:ns3="5637b85f-05ae-42d6-879b-f626b8425ad6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="297f3d60b40623b667fd0c512303efcc" ns2:_="" ns3:_="">
     <xsd:import namespace="018a9009-0ad3-4c01-a706-708408b93adc"/>
@@ -89509,27 +89529,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{332ED7EA-0DDD-44D8-B055-2DFA98457FF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5637b85f-05ae-42d6-879b-f626b8425ad6"/>
+    <ds:schemaRef ds:uri="018a9009-0ad3-4c01-a706-708408b93adc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5637b85f-05ae-42d6-879b-f626b8425ad6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="018a9009-0ad3-4c01-a706-708408b93adc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9355203E-2005-43A7-9D0A-1E4A6CF6B6F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F5BF12E-605E-41A6-9657-C3F95C26F430}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -89546,23 +89565,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9355203E-2005-43A7-9D0A-1E4A6CF6B6F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{332ED7EA-0DDD-44D8-B055-2DFA98457FF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5637b85f-05ae-42d6-879b-f626b8425ad6"/>
-    <ds:schemaRef ds:uri="018a9009-0ad3-4c01-a706-708408b93adc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>